<commit_message>
Polishing and wf doc updates
</commit_message>
<xml_diff>
--- a/data input/Abundance/AbundanceData.xlsx
+++ b/data input/Abundance/AbundanceData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/RunForecast_HoodRiver/Data input/Abundance/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mthoodenvironmental-my.sharepoint.com/personal/mark_roes_mthoodenvironmental_com/Documents/Git/RunForecast_HoodRiver/data input/Abundance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{3D52ED15-CB3B-4CBF-8AA0-423B0E4E1065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B30A83CC-939F-4048-BEF2-31D44DB53788}"/>
+  <xr:revisionPtr revIDLastSave="168" documentId="8_{3D52ED15-CB3B-4CBF-8AA0-423B0E4E1065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9BB999E-A024-40C6-B674-1B138F7EDE16}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{33466D73-0B07-4ED9-B066-F28C9CBB8D32}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33466D73-0B07-4ED9-B066-F28C9CBB8D32}"/>
   </bookViews>
   <sheets>
     <sheet name="Adult" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Year</t>
   </si>
@@ -58,19 +58,10 @@
     <t>NOR STHD</t>
   </si>
   <si>
-    <t>NOR STHD (from CTWS 2019)</t>
-  </si>
-  <si>
-    <t>NOR STHD (from forecasting sheet)</t>
-  </si>
-  <si>
     <t>SPCH BON</t>
   </si>
   <si>
     <t>SPCH DALLES</t>
-  </si>
-  <si>
-    <t>NOR WSTHD returns</t>
   </si>
   <si>
     <t>SSTHD BON</t>
@@ -164,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,9 +207,6 @@
       <alignment horizontal="centerContinuous"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -274,6 +262,10 @@
 </file>
 
 <file path=xl/persons/person16.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person17.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -609,7 +601,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H32"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -633,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -657,16 +649,16 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1027,7 +1019,7 @@
       <c r="E12" s="1">
         <v>549</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="1">
         <v>72</v>
       </c>
       <c r="G12" s="1">
@@ -1355,10 +1347,10 @@
       <c r="E20" s="3">
         <v>318</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="1">
         <v>123</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="1">
         <v>4</v>
       </c>
       <c r="H20" s="1">
@@ -1397,7 +1389,7 @@
       <c r="F21" s="4">
         <v>198</v>
       </c>
-      <c r="G21" s="16"/>
+      <c r="G21" s="1"/>
       <c r="H21" s="1">
         <v>1377</v>
       </c>
@@ -1434,7 +1426,7 @@
       <c r="F22" s="5">
         <v>332</v>
       </c>
-      <c r="G22" s="16"/>
+      <c r="G22" s="1"/>
       <c r="H22" s="1">
         <v>690</v>
       </c>
@@ -1808,688 +1800,495 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124257A0-1BC7-4538-BD20-A14703465672}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="8" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1989</v>
       </c>
-      <c r="H2" s="1">
+      <c r="D2" s="1">
         <v>22292</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1990</v>
       </c>
-      <c r="H3" s="13">
+      <c r="D3" s="13">
         <v>8121.1</v>
       </c>
-      <c r="I3" s="1">
-        <v>15207</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1991</v>
       </c>
-      <c r="H4" s="13">
+      <c r="D4" s="13">
         <v>7196.8</v>
       </c>
-      <c r="I4" s="1">
-        <v>7659</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1992</v>
       </c>
-      <c r="C5">
+      <c r="B5">
         <v>38034</v>
       </c>
-      <c r="H5" s="13">
+      <c r="D5" s="13">
         <v>4357.7</v>
       </c>
-      <c r="I5" s="1">
-        <v>5777</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1993</v>
       </c>
-      <c r="C6">
+      <c r="B6">
         <v>42860</v>
       </c>
-      <c r="H6" s="13">
+      <c r="D6" s="13">
         <v>6074.3</v>
       </c>
-      <c r="I6" s="1">
-        <v>5216</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1994</v>
       </c>
+      <c r="B7">
+        <v>50904</v>
+      </c>
       <c r="C7">
-        <v>50904</v>
-      </c>
-      <c r="F7">
         <f>40348+25776+23354+23893+3509+2241+2031+2078</f>
         <v>123230</v>
       </c>
-      <c r="G7">
+      <c r="D7" s="1">
         <v>9554</v>
       </c>
-      <c r="H7" s="1">
-        <v>9554</v>
-      </c>
-      <c r="I7" s="1">
-        <v>7814</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1995</v>
       </c>
+      <c r="B8">
+        <v>59837</v>
+      </c>
       <c r="C8">
-        <v>59837</v>
-      </c>
-      <c r="F8">
         <f>33469+11928+22315+10138+22869</f>
         <v>100719</v>
       </c>
-      <c r="G8">
+      <c r="D8" s="1">
         <v>5955</v>
       </c>
-      <c r="H8" s="1">
-        <v>5955</v>
-      </c>
-      <c r="I8" s="1">
-        <v>7755</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1996</v>
       </c>
+      <c r="B9">
+        <v>62136</v>
+      </c>
       <c r="C9">
-        <v>62136</v>
-      </c>
-      <c r="F9">
         <f>84900+44311</f>
         <v>129211</v>
       </c>
-      <c r="G9">
+      <c r="D9" s="1">
         <v>8755</v>
       </c>
-      <c r="H9" s="1">
-        <v>8755</v>
-      </c>
-      <c r="I9" s="1">
-        <v>7355</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1997</v>
       </c>
+      <c r="B10">
+        <v>44991</v>
+      </c>
       <c r="C10">
-        <v>44991</v>
-      </c>
-      <c r="F10">
         <f>45767+55326</f>
         <v>101093</v>
       </c>
-      <c r="G10">
+      <c r="D10" s="1">
         <v>15972</v>
       </c>
-      <c r="H10" s="1">
-        <v>15972</v>
-      </c>
-      <c r="I10" s="1">
-        <v>12364</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1998</v>
       </c>
+      <c r="B11">
+        <v>63255</v>
+      </c>
       <c r="C11">
-        <v>63255</v>
-      </c>
-      <c r="F11">
         <f>62057+54541+8185</f>
         <v>124783</v>
       </c>
-      <c r="G11">
+      <c r="D11" s="1">
         <v>31035</v>
       </c>
-      <c r="H11" s="1">
-        <v>31035</v>
-      </c>
-      <c r="I11" s="1">
-        <v>23504</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1999</v>
       </c>
+      <c r="B12">
+        <v>50879</v>
+      </c>
       <c r="C12">
-        <v>50879</v>
-      </c>
-      <c r="F12">
         <f>25319+26503+19513+19675+30409</f>
         <v>121419</v>
       </c>
-      <c r="G12">
+      <c r="D12" s="1">
         <v>23942</v>
       </c>
-      <c r="H12" s="1">
-        <v>23942</v>
-      </c>
-      <c r="I12" s="1">
-        <v>27489</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2000</v>
       </c>
+      <c r="B13">
+        <v>62921</v>
+      </c>
       <c r="C13">
-        <v>62921</v>
-      </c>
-      <c r="F13">
         <f>33282+31052+19865+18566+15322+15164+4160</f>
         <v>137411</v>
       </c>
-      <c r="G13">
+      <c r="D13" s="1">
         <v>19266</v>
       </c>
-      <c r="H13" s="1">
-        <v>19266</v>
-      </c>
-      <c r="I13" s="1">
-        <v>21604</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2001</v>
       </c>
+      <c r="B14">
+        <v>51433</v>
+      </c>
       <c r="C14">
-        <v>51433</v>
-      </c>
-      <c r="F14">
         <f>25322+15650+26279+15387+30646+15+4481+1997+4556+2030</f>
         <v>126363</v>
       </c>
-      <c r="G14">
+      <c r="D14" s="1">
         <v>6804</v>
       </c>
-      <c r="H14" s="1">
-        <v>6804</v>
-      </c>
-      <c r="I14" s="1">
-        <v>13035</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2002</v>
       </c>
+      <c r="B15">
+        <v>59621</v>
+      </c>
       <c r="C15">
-        <v>59621</v>
-      </c>
-      <c r="F15">
         <f>28872+18480+27975+18601+31932+285+1861</f>
         <v>128006</v>
       </c>
-      <c r="G15">
+      <c r="D15" s="1">
         <v>12290</v>
       </c>
-      <c r="H15" s="1">
-        <v>12290</v>
-      </c>
-      <c r="I15" s="1">
-        <v>9547</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2003</v>
       </c>
+      <c r="B16">
+        <v>78451</v>
+      </c>
       <c r="C16">
-        <v>78451</v>
-      </c>
-      <c r="F16">
         <f>24460+19975+18687+20072+29650+36+91+65</f>
         <v>113036</v>
       </c>
-      <c r="G16">
+      <c r="D16" s="1">
         <v>14460</v>
       </c>
-      <c r="H16" s="1">
-        <v>14460</v>
-      </c>
-      <c r="I16" s="1">
-        <v>13375</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2004</v>
       </c>
+      <c r="B17">
+        <v>36819</v>
+      </c>
       <c r="C17">
-        <v>36819</v>
-      </c>
-      <c r="F17">
         <f>15164+9515+7182+8987+4990+6257+311+1862+15409+9723+7184+9141+4993+6375+312+1863+32746</f>
         <v>142014</v>
       </c>
-      <c r="G17">
+      <c r="D17" s="1">
         <v>15042</v>
       </c>
-      <c r="H17" s="1">
-        <v>15042</v>
-      </c>
-      <c r="I17" s="1">
-        <v>14751</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2005</v>
       </c>
+      <c r="B18">
+        <v>36523</v>
+      </c>
       <c r="C18">
-        <v>36523</v>
-      </c>
-      <c r="F18">
         <f>31578+32746+544+18875+734+25499+600+772+17944+812+2226+23150+45+58+1351+90+247+2567</f>
         <v>159838</v>
       </c>
-      <c r="G18">
+      <c r="D18" s="1">
         <v>21484</v>
       </c>
-      <c r="H18" s="1">
-        <v>21484</v>
-      </c>
-      <c r="I18" s="1">
-        <v>18263</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2006</v>
       </c>
+      <c r="B19">
+        <v>64736</v>
+      </c>
       <c r="C19">
-        <v>64736</v>
-      </c>
-      <c r="F19">
         <f>30143+68320</f>
         <v>98463</v>
       </c>
-      <c r="G19">
+      <c r="D19" s="1">
         <v>8395</v>
       </c>
-      <c r="H19" s="1">
-        <v>8395</v>
-      </c>
-      <c r="I19" s="1">
-        <v>14940</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>2007</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20">
+      <c r="B20">
         <v>59624</v>
       </c>
-      <c r="F20" s="9">
+      <c r="C20" s="9">
         <v>127829</v>
       </c>
-      <c r="G20">
+      <c r="D20" s="1">
         <v>4316</v>
       </c>
-      <c r="H20" s="1">
-        <v>4316</v>
-      </c>
-      <c r="I20" s="1">
-        <v>6356</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>2008</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21">
+      <c r="B21">
         <v>47347</v>
       </c>
-      <c r="F21" s="9">
+      <c r="C21" s="9">
         <v>68426</v>
       </c>
-      <c r="G21">
+      <c r="D21" s="1">
         <v>16080</v>
       </c>
-      <c r="H21" s="1">
-        <v>16080</v>
-      </c>
-      <c r="I21" s="1">
-        <v>10198</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>2009</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22">
+      <c r="B22">
         <v>50995</v>
       </c>
-      <c r="F22" s="9">
+      <c r="C22" s="9">
         <v>126660</v>
       </c>
-      <c r="G22">
+      <c r="D22" s="1">
         <v>9317</v>
       </c>
-      <c r="H22" s="1">
-        <v>9317</v>
-      </c>
-      <c r="I22" s="1">
-        <v>12699</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>2010</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23">
+      <c r="B23">
         <v>54459</v>
       </c>
-      <c r="F23" s="10">
+      <c r="C23" s="10">
         <v>158762</v>
       </c>
-      <c r="G23">
+      <c r="D23" s="1">
         <v>16810</v>
       </c>
-      <c r="H23" s="1">
-        <v>16810</v>
-      </c>
-      <c r="I23" s="1">
-        <v>13064</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>2011</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24">
+      <c r="B24">
         <v>55303</v>
       </c>
-      <c r="F24" s="10">
+      <c r="C24" s="10">
         <v>149756</v>
       </c>
-      <c r="G24">
+      <c r="D24" s="1">
         <v>18298</v>
       </c>
-      <c r="H24" s="1">
-        <v>18298</v>
-      </c>
-      <c r="I24" s="1">
-        <v>17554</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>2012</v>
       </c>
-      <c r="B25" s="8"/>
-      <c r="C25">
+      <c r="B25">
         <v>51987</v>
       </c>
-      <c r="F25" s="11">
+      <c r="C25" s="11">
         <v>165448</v>
       </c>
-      <c r="G25">
-        <v>18298</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="D25" s="1">
         <v>16243</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>2013</v>
       </c>
-      <c r="B26" s="8"/>
-      <c r="C26">
+      <c r="B26">
         <v>53235</v>
       </c>
-      <c r="F26" s="10">
+      <c r="C26" s="10">
         <v>176235</v>
       </c>
-      <c r="G26">
-        <v>42220</v>
-      </c>
-      <c r="H26" s="1">
+      <c r="D26" s="1">
         <v>39241</v>
       </c>
-      <c r="I26" s="1">
-        <v>27742</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>2014</v>
       </c>
-      <c r="B27" s="8"/>
-      <c r="C27">
+      <c r="B27">
         <v>55531</v>
       </c>
-      <c r="F27" s="10">
+      <c r="C27" s="10">
         <v>153308</v>
       </c>
-      <c r="G27">
-        <v>18305</v>
-      </c>
-      <c r="H27" s="1">
+      <c r="D27" s="1">
         <v>23150</v>
       </c>
-      <c r="I27" s="1">
-        <v>31196</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>2015</v>
       </c>
-      <c r="B28" s="8"/>
-      <c r="C28">
+      <c r="B28">
         <v>46538</v>
       </c>
-      <c r="F28" s="10">
+      <c r="C28" s="10">
         <v>107747</v>
       </c>
-      <c r="G28">
-        <v>26273</v>
-      </c>
-      <c r="H28" s="1">
+      <c r="D28" s="1">
         <v>29731</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>2016</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29">
+      <c r="B29">
         <v>54981</v>
       </c>
-      <c r="F29" s="10">
+      <c r="C29" s="10">
         <v>179987</v>
       </c>
-      <c r="G29">
-        <v>22705</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="D29" s="1">
         <v>23373</v>
       </c>
-      <c r="I29" s="1">
-        <v>26552</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>2017</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30">
+      <c r="B30">
         <v>46538</v>
       </c>
-      <c r="F30" s="10">
+      <c r="C30" s="10">
         <v>172882</v>
       </c>
-      <c r="G30">
-        <v>17318</v>
-      </c>
-      <c r="H30" s="1">
+      <c r="D30" s="1">
         <v>20275</v>
       </c>
-      <c r="I30" s="1">
-        <v>21824</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>2018</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31">
+      <c r="B31">
         <v>54981</v>
       </c>
-      <c r="F31" s="10">
+      <c r="C31" s="10">
         <v>199298</v>
       </c>
-      <c r="G31">
-        <v>16930</v>
-      </c>
-      <c r="H31" s="1">
+      <c r="D31" s="1">
         <v>19947</v>
       </c>
-      <c r="I31" s="1">
-        <v>20111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>2019</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32">
+      <c r="B32">
         <v>54931</v>
       </c>
-      <c r="F32" s="10">
+      <c r="C32" s="10">
         <v>192131</v>
       </c>
-      <c r="H32" s="1">
+      <c r="D32" s="1">
         <v>20898</v>
       </c>
-      <c r="I32" s="1">
-        <v>20423</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>2020</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33">
+      <c r="B33">
         <v>50680</v>
       </c>
-      <c r="F33" s="10">
+      <c r="C33" s="10">
         <v>213405</v>
       </c>
-      <c r="H33" s="1">
+      <c r="D33" s="1">
         <v>26535</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>2021</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34">
+      <c r="B34">
         <v>48195</v>
       </c>
-      <c r="F34" s="12">
+      <c r="C34" s="12">
         <v>249651</v>
       </c>
-      <c r="H34" s="1">
+      <c r="D34" s="1">
         <v>15224</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>2022</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35">
+      <c r="B35">
         <v>0</v>
       </c>
-      <c r="F35" s="12">
+      <c r="C35" s="12">
         <v>257820</v>
       </c>
-      <c r="H35" s="1">
+      <c r="D35" s="1">
         <v>14994</v>
       </c>
     </row>

</xml_diff>